<commit_message>
Sesionador funcional con BEES
</commit_message>
<xml_diff>
--- a/assets/credenciales.xlsx
+++ b/assets/credenciales.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +49,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,15 +57,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,74 +426,111 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="38.140625" customWidth="1" min="1" max="1"/>
     <col width="52.140625" customWidth="1" min="2" max="2"/>
-    <col width="30.42578125" customWidth="1" min="3" max="3"/>
+    <col width="111.5703125" customWidth="1" min="3" max="3"/>
     <col width="109.7109375" customWidth="1" min="4" max="4"/>
+    <col width="113.7109375" customWidth="1" min="6" max="6"/>
+    <col width="31.42578125" customWidth="1" min="7" max="7"/>
+    <col width="101.5703125" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>CORREO ELECTRÓNICO MAXICONSUMO</t>
-        </is>
-      </c>
+      <c r="A1" s="2" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>orlando.piccinini@gmail.com</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CONTRASEÑA MAXICONSUMO</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orlando.piccinini@gmail.com</t>
+          <t>NOMBRE DE USUARIO</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>CONTRASEÑA ENCRIPTADA</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CORREO ELECTRÓNICO LA SERENÍSIMA</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>G4ZUo5+ESqk=*uHYN4TpjKFbgDDtqPrJB4g==*reeacZwe0ketMw+qfHKHfA==*w29iRiGaEBbs0pHW+7F2gA==</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CONTRASEÑA LA SERENÍSIMA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Ul57wgFmazXRT6M=*6dX0P0xXwa0vWkN9v4GPGA==*3MIV+Y5Az1m3c8Bltqbhsg==*qP9bdRX4M+v781+SGYitYg==</t>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>MAXICONSUMO</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>orlando.piccinini@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>26TBDyfahsU=*kVpqWxsj5NswRl9AYd9qVw==*Ok3UyLr0xbq0hjgxP0lomw==*NepodkMzbVYH+ModcC9Sgw==</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="1" t="n"/>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>LA SERENÍSIMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>orlando.piccinini@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>7bwYIZivWO4dVRM=*mWprFGvNLOSV5+crKLSdxQ==*lhWQVj7MPOLpUA4Q8ciZ3Q==*q7T1Qa4n1CiByRrvIilD0g==</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BEES (GRAL. ALVEAR)</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>2625404916</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>ddALT7mE3UQwH+DgsjKs900=*XX5AKld2q0bF52DUbAnM8w==*75+mUm0SnqACoKlKdheVgQ==*SsCetcMJvyJU29lez1AvQA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BEES (SAN RAFAEL)</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>1158108611</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>BXDa7+m0Z3fg*sOGWT/rynsrO5dtvUe7tgw==*qAs8nFu3/+r9znWBh8KsUA==*eescdr4iBwPxuRun34hgZg==</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="C6" s="1" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Arreglada compatibilidad con el chromedriver
</commit_message>
<xml_diff>
--- a/assets/credenciales.xlsx
+++ b/assets/credenciales.xlsx
@@ -1,77 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicob\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A732A0-FD58-4139-B8D9-ED69A58DC62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2835" yWindow="2595" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>NOMBRE DE USUARIO</t>
-  </si>
-  <si>
-    <t>CONTRASEÑA ENCRIPTADA</t>
-  </si>
-  <si>
-    <t>MAXICONSUMO</t>
-  </si>
-  <si>
-    <t>LA SERENÍSIMA</t>
-  </si>
-  <si>
-    <t>BEES (GRAL. ALVEAR)</t>
-  </si>
-  <si>
-    <t>BEES (SAN RAFAEL)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -106,25 +78,84 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -390,66 +421,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="111.5703125" customWidth="1"/>
-    <col min="4" max="4" width="109.7109375" customWidth="1"/>
-    <col min="6" max="6" width="113.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="101.5703125" customWidth="1"/>
+    <col width="38.140625" customWidth="1" min="1" max="1"/>
+    <col width="52.140625" customWidth="1" min="2" max="2"/>
+    <col width="111.5703125" customWidth="1" min="3" max="3"/>
+    <col width="109.7109375" customWidth="1" min="4" max="4"/>
+    <col width="113.7109375" customWidth="1" min="6" max="6"/>
+    <col width="31.42578125" customWidth="1" min="7" max="7"/>
+    <col width="101.5703125" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>NOMBRE DE USUARIO</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>CONTRASEÑA ENCRIPTADA</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>MAXICONSUMO</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>orlando.piccinini@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>V8+B1Y/IGZE=*Ny4e0A4rSWak9DU38ZoEXw==*f0oPqWckkaxVD3OG4zU9GA==*Spb41E7tS9SDFfrH4qga+A==</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>LA SERENÍSIMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BEES (GRAL. ALVEAR)</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BEES (SAN RAFAEL)</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+    <row r="6">
+      <c r="C6" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>